<commit_message>
Name swap "Bouquets" and "Serenade"
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material_11thanniversary.xlsx
+++ b/misc/genmaterial/material_11thanniversary.xlsx
@@ -1668,19 +1668,19 @@
     <t>Mongooses</t>
   </si>
   <si>
+    <t>Serenade</t>
+  </si>
+  <si>
+    <t>Draw [🌅 1 🃏] [☀️ 2 🃏🃏] [🌙 1 🃏]. Place 1 🃏 on your deck.</t>
+  </si>
+  <si>
+    <t>Selecting Contracts</t>
+  </si>
+  <si>
+    <t>Toss any 1 🃏 of the top [🌅 2 🃏🃏] [☀️ 4 🃏🃏🃏] [🌙 1 🃏] of your discard. Place the rest on your deck in any order.</t>
+  </si>
+  <si>
     <t>Bouquets</t>
-  </si>
-  <si>
-    <t>Draw [🌅 1 🃏] [☀️ 2 🃏🃏] [🌙 1 🃏]. Place 1 🃏 on your deck.</t>
-  </si>
-  <si>
-    <t>Selecting Contracts</t>
-  </si>
-  <si>
-    <t>Toss any 1 🃏 of the top [🌅 2 🃏🃏] [☀️ 4 🃏🃏🃏] [🌙 1 🃏] of your discard. Place the rest on your deck in any order.</t>
-  </si>
-  <si>
-    <t>Serenade</t>
   </si>
   <si>
     <t>Take 1 🃏 from [🌅 your stall] [☀️ an opponent's stall] [🌙 the market]. Place this 🃏 in its place.</t>

</xml_diff>

<commit_message>
Rename matchingColours -> colourSwap
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material_11thanniversary.xlsx
+++ b/misc/genmaterial/material_11thanniversary.xlsx
@@ -719,7 +719,7 @@
     <t>You may toss 1 🃏 from the supply. You may swap 1 animalfolk 🃏 with the top 🃏 of the bin.</t>
   </si>
   <si>
-    <t>Matching Colours</t>
+    <t>Colour Swap</t>
   </si>
   <si>
     <t>Swap 1 animalfolk 🃏 with 1 🃏 of equal value from any player's stall.</t>
@@ -1434,7 +1434,7 @@
     <t>Roll ❇️✳️. Swap 2 🃏🃏 from any player's [source] with as many 🃏🃏 from a different player's [destination].</t>
   </si>
   <si>
-    <t>Fresh Start</t>
+    <t>Souvenirs</t>
   </si>
   <si>
     <t>Draw 🃏🃏🃏 from the supply equal to the number of players. Give 1 of them to each player.</t>
@@ -7143,7 +7143,7 @@
       <c r="A103" s="22">
         <v>101.0</v>
       </c>
-      <c r="B103" s="23" t="s">
+      <c r="B103" s="22" t="s">
         <v>228</v>
       </c>
       <c r="C103" s="22" t="s">
@@ -10501,7 +10501,7 @@
       <c r="A181" s="43">
         <v>179.0</v>
       </c>
-      <c r="B181" s="46" t="s">
+      <c r="B181" s="43" t="s">
         <v>400</v>
       </c>
       <c r="C181" s="43" t="s">

</xml_diff>

<commit_message>
Rename CT_DEPRECATED_RIGOROUSCHRONICLER -> CT_VORACIOUSCONSUMER
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material_11thanniversary.xlsx
+++ b/misc/genmaterial/material_11thanniversary.xlsx
@@ -203,7 +203,7 @@
     <t>Take the top 🃏 of another player's deck or discard.</t>
   </si>
   <si>
-    <t>Stashing vendor</t>
+    <t>Stashing Vendor</t>
   </si>
   <si>
     <t>When used to build, you can include junk 🃏🃏🃏.</t>
@@ -3731,7 +3731,7 @@
       <c r="A26" s="6">
         <v>24.0</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C26" s="6" t="s">

</xml_diff>

<commit_message>
Update material for tasmanian devils
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material_11thanniversary.xlsx
+++ b/misc/genmaterial/material_11thanniversary.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="572">
   <si>
     <t>type_id</t>
   </si>
@@ -11527,13 +11527,11 @@
       <c r="C204" s="58" t="s">
         <v>452</v>
       </c>
-      <c r="D204" s="58" t="s">
-        <v>17</v>
-      </c>
-      <c r="E204" s="58" t="s">
-        <v>17</v>
-      </c>
-      <c r="F204" s="59"/>
+      <c r="D204" s="58"/>
+      <c r="E204" s="58"/>
+      <c r="F204" s="58" t="s">
+        <v>17</v>
+      </c>
       <c r="G204" s="59"/>
       <c r="H204" s="60">
         <v>5.0</v>

</xml_diff>

<commit_message>
Add CT_CAPUCHINS1 and CT_CAPUCHINS2
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material_11thanniversary.xlsx
+++ b/misc/genmaterial/material_11thanniversary.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="572">
   <si>
     <t>type_id</t>
   </si>
@@ -8293,7 +8293,9 @@
       </c>
       <c r="D129" s="37"/>
       <c r="E129" s="37"/>
-      <c r="F129" s="37"/>
+      <c r="F129" s="34" t="s">
+        <v>17</v>
+      </c>
       <c r="G129" s="38"/>
       <c r="H129" s="31">
         <v>2.0</v>

</xml_diff>

<commit_message>
Rename plural to singular animalfolk card names (e.g. CT_CAPUCHINS3 -> CT_CAPUCHIN3)
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material_11thanniversary.xlsx
+++ b/misc/genmaterial/material_11thanniversary.xlsx
@@ -845,7 +845,7 @@
     <t>Spend X (1–10) to gain X/2 🟡 (rounded up).</t>
   </si>
   <si>
-    <t>Dodos 1</t>
+    <t>Dodo 1</t>
   </si>
   <si>
     <r>
@@ -878,7 +878,7 @@
     <t>Dodos</t>
   </si>
   <si>
-    <t>Dodos 2</t>
+    <t>Dodo 2</t>
   </si>
   <si>
     <r>
@@ -920,7 +920,7 @@
     </r>
   </si>
   <si>
-    <t>Dodos 3</t>
+    <t>Dodo 3</t>
   </si>
   <si>
     <r>
@@ -955,7 +955,7 @@
     </r>
   </si>
   <si>
-    <t>Dodos 4</t>
+    <t>Dodo 4</t>
   </si>
   <si>
     <r>
@@ -982,7 +982,7 @@
     </r>
   </si>
   <si>
-    <t>Dodos 5A</t>
+    <t>Dodo 5A</t>
   </si>
   <si>
     <r>
@@ -1017,7 +1017,7 @@
     </r>
   </si>
   <si>
-    <t>Dodos 5B</t>
+    <t>Dodo 5B</t>
   </si>
   <si>
     <r>
@@ -1044,7 +1044,7 @@
     </r>
   </si>
   <si>
-    <t>Capuchins 1</t>
+    <t>Capuchin 1</t>
   </si>
   <si>
     <t>Get 2 🟡. Choose an opponent to get 1 🟡.</t>
@@ -1053,19 +1053,19 @@
     <t>Capuchins</t>
   </si>
   <si>
-    <t>Capuchins 2</t>
+    <t>Capuchin 2</t>
   </si>
   <si>
     <t>Get 1 🟡.</t>
   </si>
   <si>
-    <t>Capuchins 3</t>
+    <t>Capuchin 3</t>
   </si>
   <si>
     <t>Give another player 1 🃏. Take 1 🟡 from them.</t>
   </si>
   <si>
-    <t>Capuchins 4</t>
+    <t>Capuchin 4</t>
   </si>
   <si>
     <r>
@@ -1085,7 +1085,7 @@
     </r>
   </si>
   <si>
-    <t>Capuchins 5A</t>
+    <t>Capuchin 5A</t>
   </si>
   <si>
     <r>
@@ -1105,7 +1105,7 @@
     </r>
   </si>
   <si>
-    <t>Capuchins 5B</t>
+    <t>Capuchin 5B</t>
   </si>
   <si>
     <r>
@@ -1125,7 +1125,7 @@
     </r>
   </si>
   <si>
-    <t>Olms 1</t>
+    <t>Olm 1</t>
   </si>
   <si>
     <t>You may toss 1 🃏 from the supply. When used to purchase, you may purchase the top 🃏 of the bin.</t>
@@ -1134,31 +1134,31 @@
     <t>Olms</t>
   </si>
   <si>
-    <t>Olms 2</t>
+    <t>Olm 2</t>
   </si>
   <si>
     <t>Toss any 1 animalfolk 🃏 from your discard to take the centre 🃏 from the market.</t>
   </si>
   <si>
-    <t>Olms 3</t>
+    <t>Olm 3</t>
   </si>
   <si>
     <t>Toss 1 🃏. Toss 0–2 🃏🃏 in the market.</t>
   </si>
   <si>
-    <t>Olms 4</t>
+    <t>Olm 4</t>
   </si>
   <si>
     <t>Look at the top 3 🃏🃏🃏 of an opponent's deck. You may toss 1 of them to take 1 🃏 from the market. Place all 3 🃏🃏🃏 on their discard.</t>
   </si>
   <si>
-    <t>Olms 5A</t>
+    <t>Olm 5A</t>
   </si>
   <si>
     <t>Look at 3 random 🃏🃏🃏 from an opponent. You may toss 1 of them to give 1 🃏 from the market to them.</t>
   </si>
   <si>
-    <t>Olms 5B</t>
+    <t>Olm 5B</t>
   </si>
   <si>
     <t>Place 1 🃏 from the market on each player's deck.</t>
@@ -1242,7 +1242,7 @@
     <t>Finish 3: 🃏🃏🃏 you use this turn get +1 to their value.</t>
   </si>
   <si>
-    <t>Skinks 1</t>
+    <t>Skink 1</t>
   </si>
   <si>
     <t>At the end of your turn, place the top 0–2 🃏🃏 of your discard on your deck in any order.</t>
@@ -1251,31 +1251,31 @@
     <t>Skinks</t>
   </si>
   <si>
-    <t>Skinks 2</t>
+    <t>Skink 2</t>
   </si>
   <si>
     <t>Draw 1 🃏 from the supply. At the end of your turn, toss 1 animalfolk 🃏 or this 🃏.</t>
   </si>
   <si>
-    <t>Skinks 3</t>
+    <t>Skink 3</t>
   </si>
   <si>
     <t>Draw 2 🃏🃏. At the end of your turn, toss 1 🃏.</t>
   </si>
   <si>
-    <t>Skinks 4</t>
+    <t>Skink 4</t>
   </si>
   <si>
     <t>At the end of your turn, search your deck for 1 🃏. Shuffle your deck.</t>
   </si>
   <si>
-    <t>Skinks 5A</t>
+    <t>Skink 5A</t>
   </si>
   <si>
     <t>Draw 3 🃏🃏🃏. At the end of your turn, discard 2 🃏🃏.</t>
   </si>
   <si>
-    <t>Skinks 5B</t>
+    <t>Skink 5B</t>
   </si>
   <si>
     <t>At the end of your turn, swap 1 🃏 with the top 🃏 of your discard.</t>
@@ -1443,7 +1443,7 @@
     <t>Draw 🃏🃏🃏 from the supply equal to the number of players. Give 1 of them to each player.</t>
   </si>
   <si>
-    <t>Glassfrogs 1</t>
+    <t>Glassfrog 1</t>
   </si>
   <si>
     <t>Repeat. Discard 1 🃏 to draw 1 🃏.</t>
@@ -1452,37 +1452,37 @@
     <t>Glassfrogs</t>
   </si>
   <si>
-    <t>Glassfrogs 2</t>
+    <t>Glassfrog 2</t>
   </si>
   <si>
     <t>Repeat. Look at the top 🃏 of the supply. Toss 1 🃏 in the market and place the new 🃏 in its place.</t>
   </si>
   <si>
-    <t>Glassfrogs 3</t>
+    <t>Glassfrog 3</t>
   </si>
   <si>
     <t>When this 🃏 is placed on your discard, toss any 1 🃏 from there.</t>
   </si>
   <si>
-    <t>Glassfrogs 4</t>
+    <t>Glassfrog 4</t>
   </si>
   <si>
     <t>Repeat. Search your deck for 1 🃏 to put aside. Shuffle your deck. Place the 🃏 on your deck.</t>
   </si>
   <si>
-    <t>Glassfrogs 5A</t>
+    <t>Glassfrog 5A</t>
   </si>
   <si>
     <t>Repeat. 1 random 🃏 in your hand gets +1 to its value for this turn.</t>
   </si>
   <si>
-    <t>Glassfrogs 5B</t>
+    <t>Glassfrog 5B</t>
   </si>
   <si>
     <t>Look at the top 🃏 of you deck. You may swap it with the top 🃏 of your discard.</t>
   </si>
   <si>
-    <t>Gorillas 1</t>
+    <t>Gorilla 1</t>
   </si>
   <si>
     <t>Flip and place your deck on your discard. Take the top or bottom 🃏 of your discard.</t>
@@ -1491,37 +1491,37 @@
     <t>Gorillas</t>
   </si>
   <si>
-    <t>Gorillas 2</t>
+    <t>Gorilla 2</t>
   </si>
   <si>
     <t>Discard your hand. Take 1 🃏 from the market.</t>
   </si>
   <si>
-    <t>Gorillas 3</t>
+    <t>Gorilla 3</t>
   </si>
   <si>
     <t>Toss the top 🃏 of your deck. If it was an animalfolk 🃏, draw 1 🃏 from the supply.</t>
   </si>
   <si>
-    <t>Gorillas 4</t>
+    <t>Gorilla 4</t>
   </si>
   <si>
     <t>🃏🃏🃏 you use this turn are valued 4.</t>
   </si>
   <si>
-    <t>Gorillas 5A</t>
+    <t>Gorilla 5A</t>
   </si>
   <si>
     <t>Draw 5 🃏🃏🃏. Discard 6 🃏🃏🃏.</t>
   </si>
   <si>
-    <t>Gorillas 5B</t>
+    <t>Gorilla 5B</t>
   </si>
   <si>
     <t>Toss all 🃏🃏🃏 in the market, fill it, and take 1 🃏 from there.</t>
   </si>
   <si>
-    <t>Walruses 1</t>
+    <t>Walrus 1</t>
   </si>
   <si>
     <t>When used to build, decide this 🃏 value (1–3).</t>
@@ -1530,37 +1530,37 @@
     <t>Walruses</t>
   </si>
   <si>
-    <t>Walruses 2</t>
+    <t>Walrus 2</t>
   </si>
   <si>
     <t>When you build this turn, you may include any animalfolk 🃏🃏🃏.</t>
   </si>
   <si>
-    <t>Walruses 3</t>
+    <t>Walrus 3</t>
   </si>
   <si>
     <t>When you build this turn, you may include 1 🃏 junk.</t>
   </si>
   <si>
-    <t>Walruses 4</t>
+    <t>Walrus 4</t>
   </si>
   <si>
     <t>Take any 1 🃏 of the bottom 3 🃏🃏🃏 of your discard.</t>
   </si>
   <si>
-    <t>Walruses 5A</t>
+    <t>Walrus 5A</t>
   </si>
   <si>
     <t>If you don't build this turn, hand size +2 for this turn.</t>
   </si>
   <si>
-    <t>Walruses 5B</t>
+    <t>Walrus 5B</t>
   </si>
   <si>
     <t>While this 🃏 is in your rightmost stack, your next stack can be 1 smaller or larger than usual.</t>
   </si>
   <si>
-    <t>Tasmanian Devils 1</t>
+    <t>Tasmanian Devil 1</t>
   </si>
   <si>
     <t>Look at the top 🃏 of any player's deck. You may discard it.</t>
@@ -1569,37 +1569,37 @@
     <t>Tasmanian Devils</t>
   </si>
   <si>
-    <t>Tasmanian Devils 2</t>
+    <t>Tasmanian Devil 2</t>
   </si>
   <si>
     <t>Discard 2 random 🃏🃏 from any player. They draw as many 🃏🃏.</t>
   </si>
   <si>
-    <t>Tasmanian Devils 3</t>
+    <t>Tasmanian Devil 3</t>
   </si>
   <si>
     <t>Shuffle any 2 🃏🃏 from any player's discard into their deck.</t>
   </si>
   <si>
-    <t>Tasmanian Devils 4</t>
+    <t>Tasmanian Devil 4</t>
   </si>
   <si>
     <t>Look at the top 3 🃏🃏🃏 of any player's deck and discard any of them. Shuffle their deck.</t>
   </si>
   <si>
-    <t>Tasmanian Devils 5A</t>
+    <t>Tasmanian Devil 5A</t>
   </si>
   <si>
     <t>Discard 1 random 🃏 from any player.</t>
   </si>
   <si>
-    <t>Tasmanian Devils 5B</t>
+    <t>Tasmanian Devil 5B</t>
   </si>
   <si>
     <t>Shuffle any player’s discard. They swap 5 random 🃏🃏🃏 with the top 🃏🃏🃏 of their discard.</t>
   </si>
   <si>
-    <t>Junglefowls 1</t>
+    <t>Junglefowl 1</t>
   </si>
   <si>
     <t>Draw 1 🃏 [🌅 +1 🃏].</t>
@@ -1608,31 +1608,31 @@
     <t>Junglefowls</t>
   </si>
   <si>
-    <t>Junglefowls 2</t>
+    <t>Junglefowl 2</t>
   </si>
   <si>
     <t>Draw 1 🃏 from the supply. [🌅 Hand size +3 for this turn.]</t>
   </si>
   <si>
-    <t>Junglefowls 3</t>
+    <t>Junglefowl 3</t>
   </si>
   <si>
     <t>Toss 1 🃏. [🌅 Draw 2 🃏🃏.]</t>
   </si>
   <si>
-    <t>Junglefowls 4</t>
+    <t>Junglefowl 4</t>
   </si>
   <si>
     <t>Look at the top 2 🃏🃏 [🌅 +2 🃏🃏] of your deck and take 1 of them. You may reorder the rest.</t>
   </si>
   <si>
-    <t>Junglefowls 5A</t>
+    <t>Junglefowl 5A</t>
   </si>
   <si>
     <t>Shuffle your discard. Take any 1 🃏 of the top 2 🃏🃏 [🌅 or 4 🃏🃏🃏] of your discard.</t>
   </si>
   <si>
-    <t>Junglefowls 5B</t>
+    <t>Junglefowl 5B</t>
   </si>
   <si>
     <t>Draw 1 🃏. It gets [🌅 +2] [☀️ +1] [🌙 -1] to its value for this turn.</t>
@@ -1845,19 +1845,19 @@
     <t>Mono gains 10 🟡. Acquire.</t>
   </si>
   <si>
-    <t>Dodos Mono</t>
+    <t>Dodo Mono</t>
   </si>
   <si>
     <t>Mono gains 12 🟡. Acquire. At the end of its turn, Mono discards 2 🃏🃏.</t>
   </si>
   <si>
-    <t>Capuchins Mono</t>
+    <t>Capuchin Mono</t>
   </si>
   <si>
     <t>Mono takes 1 🟡 from you. Discard 1 🃏 from your deck. If it is not junk, Mono takes it. Acquire.</t>
   </si>
   <si>
-    <t>Olms Mono</t>
+    <t>Olm Mono</t>
   </si>
   <si>
     <t>You toss 1 random animalfolk 🃏 valued 2+ to take the lowest valued 🃏 from the market.</t>
@@ -1875,7 +1875,7 @@
     <t>Next time Mono starts its turn with no Mono 🃏🃏🃏, it takes the leftmost 🃏 from the market.</t>
   </si>
   <si>
-    <t>Skinks Mono</t>
+    <t>Skink Mono</t>
   </si>
   <si>
     <t>Mono draws 2 🃏🃏. Acquire. At the end of Mono's turn, it draws 2 🃏🃏.</t>
@@ -1908,31 +1908,31 @@
     <t>Roll ❇️✳️. Look at 1 🃏 from your [source]. If it is not junk, place it into Mono's [destination]. Acquire.</t>
   </si>
   <si>
-    <t>Glassfrogs Mono</t>
+    <t>Glassfrog Mono</t>
   </si>
   <si>
     <t>Mono draws 2 🃏🃏 and discards its 2 lowest 🃏🃏. Twice. Acquire.</t>
   </si>
   <si>
-    <t>Gorillas Mono</t>
+    <t>Gorilla Mono</t>
   </si>
   <si>
     <t>🃏🃏🃏 Mono uses this turn are valued 4. Acquire.</t>
   </si>
   <si>
-    <t>Walruses Mono</t>
+    <t>Walrus Mono</t>
   </si>
   <si>
     <t>Mono can use a single animalfolk 🃏 to build a stack this turn.</t>
   </si>
   <si>
-    <t>Tasmanian Devils Mono</t>
+    <t>Shrewd Member</t>
   </si>
   <si>
     <t>You discard 1 random 🃏. Shuffle 2 junk 🃏🃏 from your discard into your deck. Acquire.</t>
   </si>
   <si>
-    <t>Junglefowls Mono</t>
+    <t>Junglefowl Mono</t>
   </si>
   <si>
     <t>Mono's hand size [🌅 +4] [☀️ +3] [🌙 -1] for this turn. Acquire.</t>

</xml_diff>

<commit_message>
Add deck selection tooltips
</commit_message>
<xml_diff>
--- a/misc/genmaterial/material_11thanniversary.xlsx
+++ b/misc/genmaterial/material_11thanniversary.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="600">
   <si>
     <t>type_id</t>
   </si>
@@ -1731,120 +1731,180 @@
     <t>animalfolk_game</t>
   </si>
   <si>
+    <t>animalfolk_flavour</t>
+  </si>
+  <si>
     <t>Swift Member</t>
   </si>
   <si>
     <t>Mono draws 3 🃏🃏🃏. Acquire.</t>
   </si>
   <si>
+    <t>Macaws help you manage your hand of cards. New players like their opportunistic nature while seasoned players use them to optimise their play.</t>
+  </si>
+  <si>
     <t>Loyal Member</t>
   </si>
   <si>
     <t>Mono takes the highest printed valued 🃏 from the market.</t>
   </si>
   <si>
+    <t>Pandas are close friends with the market keepers and benefit from that. They’re great for beginners and players wanting a more peaceful game.</t>
+  </si>
+  <si>
     <t>Wily Member</t>
   </si>
   <si>
     <t>Mono swaps 1 random 🃏 from you with 1 junk 🃏 from it. Acquire.</t>
   </si>
   <si>
+    <t>Raccoons are a great addition for players wanting some conflict. They don’t care about the definition of ‘ownership’. You have been warned!</t>
+  </si>
+  <si>
     <t>Stashing Member</t>
   </si>
   <si>
     <t>Mono can use junk 🃏🃏🃏 to build this turn.</t>
   </si>
   <si>
+    <t>No one can set up their stall faster than squirrels. Inexperienced players like these hoarders, while experts can pull off nice combos with them.</t>
+  </si>
+  <si>
     <t>Bold Member</t>
   </si>
   <si>
     <t>Roll 🐱. Swap that many 🃏🃏🃏 between the tops of your and Mono’s decks. Acquire.</t>
   </si>
   <si>
+    <t>Ocelots can give you an edge if luck is on your side. Add these to the game when you want to introduce a little havoc to your contest!</t>
+  </si>
+  <si>
     <t>Flexible Member</t>
   </si>
   <si>
     <t>If Mono's discard has no Mono 🃏🃏🃏, discard its deck. Mono plays 1 Mono 🃏 from its discard.</t>
   </si>
   <si>
+    <t>Chameleons make you play your cards as if they’re other cards in the game. They are recommended for more experienced players with long-term plans.</t>
+  </si>
+  <si>
     <t>Tireless Member</t>
   </si>
   <si>
     <t>Order 🃏🃏🃏 in the market from the highest to lowest value. Mono ignores the market's added costs this turn. Acquire.</t>
   </si>
   <si>
+    <t>Platypuses get the right cards into their hands at the right time. Rookies grasp platypuses quickly and experienced players like to try out new things with them.</t>
+  </si>
+  <si>
     <t>Steady Member</t>
   </si>
   <si>
     <t>At the start of Mono’s next turn, it takes the leftmost 🃏 from the market.</t>
   </si>
   <si>
+    <t>You need to make plans with sloths if you don’t want to waste their delayed effects. Feel free to include them even in your first game – just don’t expect to be able to unleash their full potential right away!</t>
+  </si>
+  <si>
     <t>Little Member</t>
   </si>
   <si>
     <t>Mono draws 1 🃏 from your deck. It places back its lowest 🃏. Acquire.</t>
   </si>
   <si>
+    <t>Crocodiles bully other competitors by stealing their property and making threats. Invite crocodiles if you want interaction and conflict!</t>
+  </si>
+  <si>
     <t>Cunning Member</t>
   </si>
   <si>
     <t>Mono draws 1 🃏 from its and your deck. It gives you the lower valued 🃏 of those. Acquire.</t>
   </si>
   <si>
+    <t>Foxes love to get everyone involved. Other folks are wary of their seemingly friendly gestures, but can’t resist foxes’ tempting aid. Playing with them requires skill as timing can be critical with foxes.</t>
+  </si>
+  <si>
     <t>Daring Member</t>
   </si>
   <si>
     <t>Roll 💈. Multiply the value of each 🃏 Mono uses this turn by the rolled value. Acquire.</t>
   </si>
   <si>
+    <t>No mountain is too tall or ocean too deep for polecats! These brave adventurers live for danger and aren’t afraid of taking chances. Feeling lucky?</t>
+  </si>
+  <si>
     <t>Wise Member</t>
   </si>
   <si>
     <t>If you purchased on your last turn, Mono draws 4 🃏🃏🃏. Otherwise, it draws 2 🃏🃏. Acquire.</t>
   </si>
   <si>
+    <t>Owls wait patiently for their target to make a move before making their own. They are great at adding more interaction between players and will keep you on your toes. Stay vigilant!</t>
+  </si>
+  <si>
     <t>Rigorous Member</t>
   </si>
   <si>
     <t>Mono discards all junk 🃏🃏🃏. It draws as many 🃏🃏🃏 +1. Acquire.</t>
   </si>
   <si>
+    <t>Monitors excel at manipulating their discard piles. Do you have great cards in your discard and useless junk in your deck? You can fix that in no time with the monitors!</t>
+  </si>
+  <si>
     <t>Voracious Member</t>
   </si>
   <si>
     <t>Mono tosses its lowest valued animalfolk 🃏. Mono takes the highest valued 🃏 from the market. Acquire.</t>
   </si>
   <si>
+    <t>Getting rid of old items and trying out new things is second nature to the rather impatient lemurs. Don’t get too attached to your cards and introduce them to your game!</t>
+  </si>
+  <si>
     <t>Pompous Member</t>
   </si>
   <si>
     <t>Discard 1 random 🃏 from your hand. If the 🃏 value matches any 🃏🃏🃏 in the market, Mono takes it. Acquire.</t>
   </si>
   <si>
+    <t>Magpies are choosy thieves. They try to steal only specific items and nothing more. You need to keep an eye on your opponents to utilise magpies to their full potential. For advanced players only!</t>
+  </si>
+  <si>
     <t>Carefree Member</t>
   </si>
   <si>
     <t>Swap Mono's lowest animalfolk 🃏 with 1 random animalfolk 🃏 of higher value from you. Acquire.</t>
   </si>
   <si>
+    <t>Echidnas borrow cards from everyone, but at least they always leave something as a replacement. Add them in when you want a lot of interaction between players without straight-out stealing.</t>
+  </si>
+  <si>
     <t>Arcane Member</t>
   </si>
   <si>
     <t>Roll 🐰. Mono draws 1 🃏 from [☄️: nowhere] [🪐: the supply] [✨: its deck]. Acquire.</t>
   </si>
   <si>
+    <t>Statistics and calculations or blind trust in beliefs from previous generations? Hares introduce luck, but you can do a lot to play around it with precise timing and careful preparations.</t>
+  </si>
+  <si>
     <t>Clever Member</t>
   </si>
   <si>
     <t>Mono stores the top 3 🃏🃏🃏 of its deck. Acquire.</t>
   </si>
   <si>
+    <t>Kangaroos are excellent at hiding their valuables and creating diversions for mischief makers. However, their techniques are useful even when no one is playing dirty.</t>
+  </si>
+  <si>
     <t>Avid Member</t>
   </si>
   <si>
     <t>Mono gains 10 🟡. Acquire.</t>
   </si>
   <si>
+    <t>Tuataras benefit from the riches gathered by their ancestors. You can save up gold and gain new options, including purchasing expensive cards more easily.</t>
+  </si>
+  <si>
     <t>Dodo Mono</t>
   </si>
   <si>
@@ -1869,12 +1929,18 @@
     <t>Add +1 to Mono’s highest valued animalfolk 🃏 for each junk 🃏 in its hand.</t>
   </si>
   <si>
+    <t>Penguins give you potent effects for tough situations. Their power comes at a cost which seasoned players can turn into an advantage.</t>
+  </si>
+  <si>
     <t>Impulsive Member</t>
   </si>
   <si>
     <t>Next time Mono starts its turn with no Mono 🃏🃏🃏, it takes the leftmost 🃏 from the market.</t>
   </si>
   <si>
+    <t>Turtles like to play new techniques but struggle to finish them. If you’re not careful, everything can come to a standstill. You will have to think around this.</t>
+  </si>
+  <si>
     <t>Skink Mono</t>
   </si>
   <si>
@@ -1890,6 +1956,9 @@
     <t>onMonoFailsToBuild</t>
   </si>
   <si>
+    <t>Do you have what it takes to create a plan and then execute it with precision? Master beavers to unleash awesome combos! They are recommended for a bit more experienced players.</t>
+  </si>
+  <si>
     <t>Pristine Member</t>
   </si>
   <si>
@@ -1902,12 +1971,18 @@
     <t>Place 1 junk 🃏 from Mono’s discard and 1 junk 🃏 from the junkyard on your discard. Acquire.</t>
   </si>
   <si>
+    <t>Gulls absolutely love gifting junk to their opponents to slow them down! Novices can get the hang of them pretty fast. Just be prepared for a slightly slower game.</t>
+  </si>
+  <si>
     <t>Fumbling Member</t>
   </si>
   <si>
     <t>Roll ❇️✳️. Look at 1 🃏 from your [source]. If it is not junk, place it into Mono's [destination]. Acquire.</t>
   </si>
   <si>
+    <t>Pangolins cause destruction by being so absent-minded. Even more skilled players may have trouble exploiting their potential without it backfiring.</t>
+  </si>
+  <si>
     <t>Glassfrog Mono</t>
   </si>
   <si>
@@ -1932,6 +2007,9 @@
     <t>You discard 1 random 🃏. Shuffle 2 junk 🃏🃏 from your discard into your deck. Acquire.</t>
   </si>
   <si>
+    <t>Tasmanian devils are your best bet if you want to mess up your opponents’ plans! They’re not ones to steal, but they do enhance it if you invite those that are.</t>
+  </si>
+  <si>
     <t>Junglefowl Mono</t>
   </si>
   <si>
@@ -1944,10 +2022,16 @@
     <t>Mono draws [🌅 3 🃏🃏🃏] [☀️ 4 🃏🃏🃏] [🌙 2 🃏🃏]. Acquire.</t>
   </si>
   <si>
+    <t>Mongooses work hard during the day. Managing your tempo becomes increasingly important as you try to benefit more from them than your opponents do.</t>
+  </si>
+  <si>
     <t>Stealthy Member</t>
   </si>
   <si>
     <t>[☀️ Mono draws 1 🃏 from your deck.] [🌙 Mono takes 1 random animalfolk 🃏 from you.] Acquire.</t>
+  </si>
+  <si>
+    <t>Bats appear innocent during the day, but just wait for the night to set in! Your possessions will end up either missing or destroyed by the time dawn approaches.</t>
   </si>
 </sst>
 </file>
@@ -2213,6 +2297,9 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
@@ -2243,9 +2330,6 @@
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -32671,7 +32755,7 @@
     <col customWidth="1" min="14" max="14" width="22.0"/>
     <col customWidth="1" min="15" max="15" width="22.29"/>
     <col customWidth="1" min="16" max="16" width="21.71"/>
-    <col customWidth="1" min="17" max="17" width="19.43"/>
+    <col customWidth="1" min="17" max="17" width="222.14"/>
     <col customWidth="1" min="18" max="18" width="29.0"/>
   </cols>
   <sheetData>
@@ -32724,256 +32808,268 @@
       <c r="P1" s="70" t="s">
         <v>498</v>
       </c>
-      <c r="Q1" s="2"/>
+      <c r="Q1" s="71" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="71">
+      <c r="A2" s="72">
         <v>222.0</v>
       </c>
-      <c r="B2" s="72" t="s">
-        <v>499</v>
-      </c>
-      <c r="C2" s="72" t="s">
+      <c r="B2" s="73" t="s">
         <v>500</v>
       </c>
-      <c r="D2" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73">
+      <c r="C2" s="73" t="s">
+        <v>501</v>
+      </c>
+      <c r="D2" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="73"/>
+      <c r="H2" s="74">
         <v>2.0</v>
       </c>
-      <c r="I2" s="73">
+      <c r="I2" s="74">
         <v>0.0</v>
       </c>
-      <c r="J2" s="72" t="s">
+      <c r="J2" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="74">
+      <c r="K2" s="75">
         <v>1.0</v>
       </c>
-      <c r="L2" s="75">
+      <c r="L2" s="76">
         <v>1.0</v>
       </c>
-      <c r="M2" s="75">
+      <c r="M2" s="76">
         <v>1.0</v>
       </c>
-      <c r="N2" s="75">
+      <c r="N2" s="76">
         <v>0.0</v>
       </c>
-      <c r="O2" s="75">
+      <c r="O2" s="76">
         <v>1.0</v>
       </c>
-      <c r="P2" s="76">
+      <c r="P2" s="77">
         <v>1.0</v>
       </c>
-      <c r="Q2" s="2"/>
+      <c r="Q2" s="76" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="71">
+      <c r="A3" s="72">
         <v>223.0</v>
       </c>
-      <c r="B3" s="72" t="s">
-        <v>501</v>
-      </c>
-      <c r="C3" s="72" t="s">
-        <v>502</v>
-      </c>
-      <c r="D3" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="73">
+      <c r="B3" s="73" t="s">
+        <v>503</v>
+      </c>
+      <c r="C3" s="73" t="s">
+        <v>504</v>
+      </c>
+      <c r="D3" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="74">
         <v>2.0</v>
       </c>
-      <c r="I3" s="73">
+      <c r="I3" s="74">
         <v>0.0</v>
       </c>
-      <c r="J3" s="72" t="s">
+      <c r="J3" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="74">
+      <c r="K3" s="75">
         <v>2.0</v>
       </c>
-      <c r="L3" s="75">
+      <c r="L3" s="76">
         <v>1.0</v>
       </c>
-      <c r="M3" s="75">
+      <c r="M3" s="76">
         <v>2.0</v>
       </c>
-      <c r="N3" s="75">
+      <c r="N3" s="76">
         <v>0.0</v>
       </c>
-      <c r="O3" s="75">
+      <c r="O3" s="76">
         <v>1.0</v>
       </c>
-      <c r="P3" s="76">
+      <c r="P3" s="77">
         <v>1.0</v>
       </c>
-      <c r="Q3" s="2"/>
+      <c r="Q3" s="76" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="71">
+      <c r="A4" s="72">
         <v>224.0</v>
       </c>
-      <c r="B4" s="72" t="s">
-        <v>503</v>
-      </c>
-      <c r="C4" s="77" t="s">
-        <v>504</v>
-      </c>
-      <c r="D4" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="72"/>
-      <c r="H4" s="73">
+      <c r="B4" s="73" t="s">
+        <v>506</v>
+      </c>
+      <c r="C4" s="78" t="s">
+        <v>507</v>
+      </c>
+      <c r="D4" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="73"/>
+      <c r="H4" s="74">
         <v>2.0</v>
       </c>
-      <c r="I4" s="73">
+      <c r="I4" s="74">
         <v>0.0</v>
       </c>
-      <c r="J4" s="72" t="s">
+      <c r="J4" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="74">
+      <c r="K4" s="75">
         <v>3.0</v>
       </c>
-      <c r="L4" s="75">
+      <c r="L4" s="76">
         <v>1.0</v>
       </c>
-      <c r="M4" s="75">
+      <c r="M4" s="76">
         <v>3.0</v>
       </c>
-      <c r="N4" s="75">
+      <c r="N4" s="76">
         <v>3.0</v>
       </c>
-      <c r="O4" s="75">
+      <c r="O4" s="76">
         <v>2.0</v>
       </c>
-      <c r="P4" s="76">
+      <c r="P4" s="77">
         <v>1.0</v>
       </c>
-      <c r="Q4" s="2"/>
+      <c r="Q4" s="76" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="71">
+      <c r="A5" s="72">
         <v>225.0</v>
       </c>
-      <c r="B5" s="72" t="s">
-        <v>505</v>
-      </c>
-      <c r="C5" s="72" t="s">
-        <v>506</v>
-      </c>
-      <c r="D5" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="73">
+      <c r="B5" s="73" t="s">
+        <v>509</v>
+      </c>
+      <c r="C5" s="73" t="s">
+        <v>510</v>
+      </c>
+      <c r="D5" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="74">
         <v>2.0</v>
       </c>
-      <c r="I5" s="73">
+      <c r="I5" s="74">
         <v>0.0</v>
       </c>
-      <c r="J5" s="72" t="s">
+      <c r="J5" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="K5" s="74">
+      <c r="K5" s="75">
         <v>4.0</v>
       </c>
-      <c r="L5" s="75">
+      <c r="L5" s="76">
         <v>1.0</v>
       </c>
-      <c r="M5" s="75">
+      <c r="M5" s="76">
         <v>2.0</v>
       </c>
-      <c r="N5" s="75">
+      <c r="N5" s="76">
         <v>0.0</v>
       </c>
-      <c r="O5" s="75">
+      <c r="O5" s="76">
         <v>1.0</v>
       </c>
-      <c r="P5" s="76">
+      <c r="P5" s="77">
         <v>1.0</v>
       </c>
-      <c r="Q5" s="2"/>
+      <c r="Q5" s="76" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="71">
+      <c r="A6" s="72">
         <v>226.0</v>
       </c>
-      <c r="B6" s="72" t="s">
-        <v>507</v>
-      </c>
-      <c r="C6" s="72" t="s">
-        <v>508</v>
-      </c>
-      <c r="D6" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="72"/>
-      <c r="H6" s="73">
+      <c r="B6" s="73" t="s">
+        <v>512</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>513</v>
+      </c>
+      <c r="D6" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="73"/>
+      <c r="H6" s="74">
         <v>2.0</v>
       </c>
-      <c r="I6" s="73">
+      <c r="I6" s="74">
         <v>0.0</v>
       </c>
-      <c r="J6" s="72" t="s">
+      <c r="J6" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="K6" s="74">
+      <c r="K6" s="75">
         <v>5.0</v>
       </c>
-      <c r="L6" s="75">
+      <c r="L6" s="76">
         <v>2.0</v>
       </c>
-      <c r="M6" s="75">
+      <c r="M6" s="76">
         <v>3.0</v>
       </c>
-      <c r="N6" s="75">
+      <c r="N6" s="76">
         <v>2.0</v>
       </c>
-      <c r="O6" s="75">
+      <c r="O6" s="76">
         <v>3.0</v>
       </c>
-      <c r="P6" s="76">
+      <c r="P6" s="77">
         <v>1.0</v>
       </c>
-      <c r="Q6" s="2"/>
+      <c r="Q6" s="76" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="78">
+      <c r="A7" s="79">
         <v>227.0</v>
       </c>
       <c r="B7" s="67" t="s">
-        <v>509</v>
-      </c>
-      <c r="C7" s="79" t="s">
-        <v>510</v>
+        <v>515</v>
+      </c>
+      <c r="C7" s="80" t="s">
+        <v>516</v>
       </c>
       <c r="D7" s="67" t="s">
         <v>17</v>
@@ -32983,287 +33079,299 @@
       </c>
       <c r="F7" s="67"/>
       <c r="G7" s="67"/>
-      <c r="H7" s="80">
+      <c r="H7" s="81">
         <v>2.0</v>
       </c>
-      <c r="I7" s="80">
+      <c r="I7" s="81">
         <v>0.0</v>
       </c>
       <c r="J7" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="K7" s="81">
+      <c r="K7" s="82">
         <v>6.0</v>
       </c>
-      <c r="L7" s="82">
+      <c r="L7" s="71">
         <v>3.0</v>
       </c>
-      <c r="M7" s="82">
+      <c r="M7" s="71">
         <v>2.0</v>
       </c>
-      <c r="N7" s="82">
+      <c r="N7" s="71">
         <v>0.0</v>
       </c>
-      <c r="O7" s="82">
+      <c r="O7" s="71">
         <v>1.0</v>
       </c>
       <c r="P7" s="83">
         <v>1.0</v>
       </c>
-      <c r="Q7" s="2"/>
+      <c r="Q7" s="71" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="71">
+      <c r="A8" s="72">
         <v>228.0</v>
       </c>
       <c r="B8" s="84" t="s">
-        <v>511</v>
-      </c>
-      <c r="C8" s="77" t="s">
-        <v>512</v>
-      </c>
-      <c r="D8" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="72"/>
-      <c r="H8" s="73">
+        <v>518</v>
+      </c>
+      <c r="C8" s="78" t="s">
+        <v>519</v>
+      </c>
+      <c r="D8" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="73"/>
+      <c r="H8" s="74">
         <v>2.0</v>
       </c>
-      <c r="I8" s="73">
+      <c r="I8" s="74">
         <v>0.0</v>
       </c>
-      <c r="J8" s="72" t="s">
+      <c r="J8" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="K8" s="74">
+      <c r="K8" s="75">
         <v>7.0</v>
       </c>
-      <c r="L8" s="75">
+      <c r="L8" s="76">
         <v>1.0</v>
       </c>
-      <c r="M8" s="75">
+      <c r="M8" s="76">
         <v>1.0</v>
       </c>
-      <c r="N8" s="75">
+      <c r="N8" s="76">
         <v>0.0</v>
       </c>
-      <c r="O8" s="75">
+      <c r="O8" s="76">
         <v>1.0</v>
       </c>
       <c r="P8" s="85">
         <v>2.0</v>
       </c>
-      <c r="Q8" s="2"/>
+      <c r="Q8" s="76" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="71">
+      <c r="A9" s="72">
         <v>229.0</v>
       </c>
       <c r="B9" s="86" t="s">
-        <v>513</v>
-      </c>
-      <c r="C9" s="72" t="s">
-        <v>514</v>
-      </c>
-      <c r="D9" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72" t="s">
+        <v>521</v>
+      </c>
+      <c r="C9" s="73" t="s">
+        <v>522</v>
+      </c>
+      <c r="D9" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="H9" s="73">
+      <c r="H9" s="74">
         <v>2.0</v>
       </c>
-      <c r="I9" s="73">
+      <c r="I9" s="74">
         <v>0.0</v>
       </c>
       <c r="J9" s="87" t="s">
         <v>111</v>
       </c>
-      <c r="K9" s="74">
+      <c r="K9" s="75">
         <v>8.0</v>
       </c>
-      <c r="L9" s="75">
+      <c r="L9" s="76">
         <v>2.0</v>
       </c>
-      <c r="M9" s="75">
+      <c r="M9" s="76">
         <v>1.0</v>
       </c>
-      <c r="N9" s="75">
+      <c r="N9" s="76">
         <v>0.0</v>
       </c>
-      <c r="O9" s="75">
+      <c r="O9" s="76">
         <v>1.0</v>
       </c>
       <c r="P9" s="85">
         <v>2.0</v>
       </c>
-      <c r="Q9" s="2"/>
+      <c r="Q9" s="76" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="71">
+      <c r="A10" s="72">
         <v>230.0</v>
       </c>
       <c r="B10" s="84" t="s">
-        <v>515</v>
-      </c>
-      <c r="C10" s="72" t="s">
-        <v>516</v>
-      </c>
-      <c r="D10" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="72"/>
-      <c r="H10" s="73">
+        <v>524</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>525</v>
+      </c>
+      <c r="D10" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="73"/>
+      <c r="H10" s="74">
         <v>2.0</v>
       </c>
-      <c r="I10" s="73">
+      <c r="I10" s="74">
         <v>0.0</v>
       </c>
       <c r="J10" s="87" t="s">
         <v>124</v>
       </c>
-      <c r="K10" s="74">
+      <c r="K10" s="75">
         <v>9.0</v>
       </c>
-      <c r="L10" s="75">
+      <c r="L10" s="76">
         <v>2.0</v>
       </c>
-      <c r="M10" s="75">
+      <c r="M10" s="76">
         <v>3.0</v>
       </c>
-      <c r="N10" s="75">
+      <c r="N10" s="76">
         <v>3.0</v>
       </c>
-      <c r="O10" s="75">
+      <c r="O10" s="76">
         <v>1.0</v>
       </c>
       <c r="P10" s="85">
         <v>2.0</v>
       </c>
-      <c r="Q10" s="2"/>
+      <c r="Q10" s="76" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="71">
+      <c r="A11" s="72">
         <v>231.0</v>
       </c>
       <c r="B11" s="86" t="s">
-        <v>517</v>
-      </c>
-      <c r="C11" s="72" t="s">
-        <v>518</v>
-      </c>
-      <c r="D11" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="72"/>
-      <c r="H11" s="73">
+        <v>527</v>
+      </c>
+      <c r="C11" s="73" t="s">
+        <v>528</v>
+      </c>
+      <c r="D11" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="73"/>
+      <c r="H11" s="74">
         <v>2.0</v>
       </c>
-      <c r="I11" s="73">
+      <c r="I11" s="74">
         <v>0.0</v>
       </c>
       <c r="J11" s="87" t="s">
         <v>137</v>
       </c>
-      <c r="K11" s="74">
+      <c r="K11" s="75">
         <v>10.0</v>
       </c>
-      <c r="L11" s="75">
+      <c r="L11" s="76">
         <v>3.0</v>
       </c>
-      <c r="M11" s="75">
+      <c r="M11" s="76">
         <v>3.0</v>
       </c>
-      <c r="N11" s="75">
+      <c r="N11" s="76">
         <v>2.0</v>
       </c>
-      <c r="O11" s="75">
+      <c r="O11" s="76">
         <v>2.0</v>
       </c>
       <c r="P11" s="85">
         <v>2.0</v>
       </c>
-      <c r="Q11" s="2"/>
+      <c r="Q11" s="76" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="71">
+      <c r="A12" s="72">
         <v>232.0</v>
       </c>
       <c r="B12" s="84" t="s">
-        <v>519</v>
-      </c>
-      <c r="C12" s="77" t="s">
-        <v>520</v>
-      </c>
-      <c r="D12" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="72"/>
-      <c r="H12" s="73">
+        <v>530</v>
+      </c>
+      <c r="C12" s="78" t="s">
+        <v>531</v>
+      </c>
+      <c r="D12" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="73"/>
+      <c r="H12" s="74">
         <v>2.0</v>
       </c>
-      <c r="I12" s="73">
+      <c r="I12" s="74">
         <v>0.0</v>
       </c>
       <c r="J12" s="87" t="s">
         <v>150</v>
       </c>
-      <c r="K12" s="74">
+      <c r="K12" s="75">
         <v>11.0</v>
       </c>
-      <c r="L12" s="75">
+      <c r="L12" s="76">
         <v>1.0</v>
       </c>
-      <c r="M12" s="75">
+      <c r="M12" s="76">
         <v>2.0</v>
       </c>
-      <c r="N12" s="75">
+      <c r="N12" s="76">
         <v>0.0</v>
       </c>
-      <c r="O12" s="75">
+      <c r="O12" s="76">
         <v>3.0</v>
       </c>
       <c r="P12" s="85">
         <v>2.0</v>
       </c>
-      <c r="Q12" s="2"/>
+      <c r="Q12" s="76" t="s">
+        <v>532</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="78">
+      <c r="A13" s="79">
         <v>233.0</v>
       </c>
       <c r="B13" s="88" t="s">
-        <v>521</v>
-      </c>
-      <c r="C13" s="79" t="s">
-        <v>522</v>
+        <v>533</v>
+      </c>
+      <c r="C13" s="80" t="s">
+        <v>534</v>
       </c>
       <c r="D13" s="67" t="s">
         <v>17</v>
@@ -33275,74 +33383,76 @@
         <v>17</v>
       </c>
       <c r="G13" s="67"/>
-      <c r="H13" s="80">
+      <c r="H13" s="81">
         <v>2.0</v>
       </c>
-      <c r="I13" s="80">
+      <c r="I13" s="81">
         <v>0.0</v>
       </c>
       <c r="J13" s="89" t="s">
         <v>163</v>
       </c>
-      <c r="K13" s="81">
+      <c r="K13" s="82">
         <v>12.0</v>
       </c>
-      <c r="L13" s="82">
+      <c r="L13" s="71">
         <v>3.0</v>
       </c>
-      <c r="M13" s="82">
+      <c r="M13" s="71">
         <v>3.0</v>
       </c>
-      <c r="N13" s="82">
+      <c r="N13" s="71">
         <v>0.0</v>
       </c>
-      <c r="O13" s="82">
+      <c r="O13" s="71">
         <v>1.0</v>
       </c>
       <c r="P13" s="90">
         <v>2.0</v>
       </c>
-      <c r="Q13" s="2"/>
+      <c r="Q13" s="71" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="71">
+      <c r="A14" s="72">
         <v>234.0</v>
       </c>
-      <c r="B14" s="72" t="s">
-        <v>523</v>
-      </c>
-      <c r="C14" s="77" t="s">
-        <v>524</v>
-      </c>
-      <c r="D14" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="72"/>
-      <c r="H14" s="73">
+      <c r="B14" s="73" t="s">
+        <v>536</v>
+      </c>
+      <c r="C14" s="78" t="s">
+        <v>537</v>
+      </c>
+      <c r="D14" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="73"/>
+      <c r="H14" s="74">
         <v>2.0</v>
       </c>
-      <c r="I14" s="73">
+      <c r="I14" s="74">
         <v>0.0</v>
       </c>
       <c r="J14" s="87" t="s">
         <v>181</v>
       </c>
-      <c r="K14" s="74">
+      <c r="K14" s="75">
         <v>13.0</v>
       </c>
-      <c r="L14" s="75">
+      <c r="L14" s="76">
         <v>1.0</v>
       </c>
-      <c r="M14" s="75">
+      <c r="M14" s="76">
         <v>1.0</v>
       </c>
-      <c r="N14" s="75">
+      <c r="N14" s="76">
         <v>0.0</v>
       </c>
       <c r="O14" s="91">
@@ -33351,213 +33461,223 @@
       <c r="P14" s="92">
         <v>3.0</v>
       </c>
-      <c r="Q14" s="2"/>
+      <c r="Q14" s="76" t="s">
+        <v>538</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="71">
+      <c r="A15" s="72">
         <v>235.0</v>
       </c>
-      <c r="B15" s="72" t="s">
-        <v>525</v>
-      </c>
-      <c r="C15" s="77" t="s">
-        <v>526</v>
-      </c>
-      <c r="D15" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="72"/>
-      <c r="H15" s="73">
+      <c r="B15" s="73" t="s">
+        <v>539</v>
+      </c>
+      <c r="C15" s="78" t="s">
+        <v>540</v>
+      </c>
+      <c r="D15" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="73"/>
+      <c r="H15" s="74">
         <v>2.0</v>
       </c>
-      <c r="I15" s="73">
+      <c r="I15" s="74">
         <v>0.0</v>
       </c>
       <c r="J15" s="87" t="s">
         <v>194</v>
       </c>
-      <c r="K15" s="74">
+      <c r="K15" s="75">
         <v>14.0</v>
       </c>
-      <c r="L15" s="75">
+      <c r="L15" s="76">
         <v>1.0</v>
       </c>
-      <c r="M15" s="75">
+      <c r="M15" s="76">
         <v>1.0</v>
       </c>
-      <c r="N15" s="75">
+      <c r="N15" s="76">
         <v>0.0</v>
       </c>
-      <c r="O15" s="75">
+      <c r="O15" s="76">
         <v>2.0</v>
       </c>
       <c r="P15" s="92">
         <v>3.0</v>
       </c>
-      <c r="Q15" s="2"/>
+      <c r="Q15" s="76" t="s">
+        <v>541</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="71">
+      <c r="A16" s="72">
         <v>236.0</v>
       </c>
-      <c r="B16" s="72" t="s">
-        <v>527</v>
-      </c>
-      <c r="C16" s="72" t="s">
-        <v>528</v>
-      </c>
-      <c r="D16" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="72"/>
-      <c r="H16" s="73">
+      <c r="B16" s="73" t="s">
+        <v>542</v>
+      </c>
+      <c r="C16" s="73" t="s">
+        <v>543</v>
+      </c>
+      <c r="D16" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="73"/>
+      <c r="H16" s="74">
         <v>2.0</v>
       </c>
-      <c r="I16" s="73">
+      <c r="I16" s="74">
         <v>0.0</v>
       </c>
       <c r="J16" s="87" t="s">
         <v>207</v>
       </c>
-      <c r="K16" s="74">
+      <c r="K16" s="75">
         <v>15.0</v>
       </c>
-      <c r="L16" s="75">
+      <c r="L16" s="76">
         <v>3.0</v>
       </c>
-      <c r="M16" s="75">
+      <c r="M16" s="76">
         <v>3.0</v>
       </c>
-      <c r="N16" s="75">
+      <c r="N16" s="76">
         <v>3.0</v>
       </c>
-      <c r="O16" s="75">
+      <c r="O16" s="76">
         <v>2.0</v>
       </c>
       <c r="P16" s="92">
         <v>3.0</v>
       </c>
-      <c r="Q16" s="2"/>
+      <c r="Q16" s="76" t="s">
+        <v>544</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="71">
+      <c r="A17" s="72">
         <v>237.0</v>
       </c>
-      <c r="B17" s="72" t="s">
-        <v>529</v>
-      </c>
-      <c r="C17" s="77" t="s">
-        <v>530</v>
-      </c>
-      <c r="D17" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="72"/>
-      <c r="H17" s="73">
+      <c r="B17" s="73" t="s">
+        <v>545</v>
+      </c>
+      <c r="C17" s="78" t="s">
+        <v>546</v>
+      </c>
+      <c r="D17" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="73"/>
+      <c r="H17" s="74">
         <v>2.0</v>
       </c>
-      <c r="I17" s="73">
+      <c r="I17" s="74">
         <v>0.0</v>
       </c>
       <c r="J17" s="87" t="s">
         <v>220</v>
       </c>
-      <c r="K17" s="74">
+      <c r="K17" s="75">
         <v>16.0</v>
       </c>
-      <c r="L17" s="75">
+      <c r="L17" s="76">
         <v>2.0</v>
       </c>
-      <c r="M17" s="75">
+      <c r="M17" s="76">
         <v>3.0</v>
       </c>
-      <c r="N17" s="75">
+      <c r="N17" s="76">
         <v>1.0</v>
       </c>
-      <c r="O17" s="75">
+      <c r="O17" s="76">
         <v>2.0</v>
       </c>
       <c r="P17" s="92">
         <v>3.0</v>
       </c>
-      <c r="Q17" s="2"/>
+      <c r="Q17" s="76" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="71">
+      <c r="A18" s="72">
         <v>238.0</v>
       </c>
-      <c r="B18" s="72" t="s">
-        <v>531</v>
-      </c>
-      <c r="C18" s="72" t="s">
-        <v>532</v>
-      </c>
-      <c r="D18" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="72"/>
-      <c r="H18" s="73">
+      <c r="B18" s="73" t="s">
+        <v>548</v>
+      </c>
+      <c r="C18" s="73" t="s">
+        <v>549</v>
+      </c>
+      <c r="D18" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="73"/>
+      <c r="H18" s="74">
         <v>2.0</v>
       </c>
-      <c r="I18" s="73">
+      <c r="I18" s="74">
         <v>0.0</v>
       </c>
       <c r="J18" s="87" t="s">
         <v>233</v>
       </c>
-      <c r="K18" s="74">
+      <c r="K18" s="75">
         <v>17.0</v>
       </c>
-      <c r="L18" s="75">
+      <c r="L18" s="76">
         <v>2.0</v>
       </c>
-      <c r="M18" s="75">
+      <c r="M18" s="76">
         <v>1.0</v>
       </c>
-      <c r="N18" s="75">
+      <c r="N18" s="76">
         <v>0.0</v>
       </c>
-      <c r="O18" s="75">
+      <c r="O18" s="76">
         <v>3.0</v>
       </c>
       <c r="P18" s="92">
         <v>3.0</v>
       </c>
-      <c r="Q18" s="2"/>
+      <c r="Q18" s="76" t="s">
+        <v>550</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="78">
+      <c r="A19" s="79">
         <v>239.0</v>
       </c>
       <c r="B19" s="67" t="s">
-        <v>533</v>
-      </c>
-      <c r="C19" s="79" t="s">
-        <v>534</v>
+        <v>551</v>
+      </c>
+      <c r="C19" s="80" t="s">
+        <v>552</v>
       </c>
       <c r="D19" s="67" t="s">
         <v>17</v>
@@ -33569,7 +33689,7 @@
         <v>17</v>
       </c>
       <c r="G19" s="67"/>
-      <c r="H19" s="80">
+      <c r="H19" s="81">
         <v>2.0</v>
       </c>
       <c r="I19" s="94">
@@ -33578,47 +33698,49 @@
       <c r="J19" s="95" t="s">
         <v>246</v>
       </c>
-      <c r="K19" s="81">
+      <c r="K19" s="82">
         <v>18.0</v>
       </c>
-      <c r="L19" s="82">
+      <c r="L19" s="71">
         <v>2.0</v>
       </c>
-      <c r="M19" s="82">
+      <c r="M19" s="71">
         <v>1.0</v>
       </c>
-      <c r="N19" s="82">
+      <c r="N19" s="71">
         <v>0.0</v>
       </c>
-      <c r="O19" s="82">
+      <c r="O19" s="71">
         <v>1.0</v>
       </c>
       <c r="P19" s="96">
         <v>3.0</v>
       </c>
-      <c r="Q19" s="2"/>
+      <c r="Q19" s="71" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="71">
+      <c r="A20" s="72">
         <v>240.0</v>
       </c>
-      <c r="B20" s="72" t="s">
-        <v>535</v>
-      </c>
-      <c r="C20" s="72" t="s">
-        <v>536</v>
-      </c>
-      <c r="D20" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="72" t="s">
+      <c r="B20" s="73" t="s">
+        <v>554</v>
+      </c>
+      <c r="C20" s="73" t="s">
+        <v>555</v>
+      </c>
+      <c r="D20" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="73" t="s">
         <v>17</v>
       </c>
       <c r="F20" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="72"/>
-      <c r="H20" s="73">
+      <c r="G20" s="73"/>
+      <c r="H20" s="74">
         <v>2.0</v>
       </c>
       <c r="I20" s="98">
@@ -33627,190 +33749,194 @@
       <c r="J20" s="99" t="s">
         <v>259</v>
       </c>
-      <c r="K20" s="74">
+      <c r="K20" s="75">
         <v>19.0</v>
       </c>
-      <c r="L20" s="75">
+      <c r="L20" s="76">
         <v>2.0</v>
       </c>
-      <c r="M20" s="75">
+      <c r="M20" s="76">
         <v>1.0</v>
       </c>
-      <c r="N20" s="75">
+      <c r="N20" s="76">
         <v>0.0</v>
       </c>
-      <c r="O20" s="75">
+      <c r="O20" s="76">
         <v>1.0</v>
       </c>
       <c r="P20" s="100">
         <v>4.0</v>
       </c>
-      <c r="Q20" s="2"/>
+      <c r="Q20" s="76" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="71">
+      <c r="A21" s="72">
         <v>241.0</v>
       </c>
-      <c r="B21" s="75" t="s">
-        <v>537</v>
-      </c>
-      <c r="C21" s="75" t="s">
-        <v>538</v>
-      </c>
-      <c r="D21" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="75" t="s">
+      <c r="B21" s="76" t="s">
+        <v>557</v>
+      </c>
+      <c r="C21" s="76" t="s">
+        <v>558</v>
+      </c>
+      <c r="D21" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="76" t="s">
         <v>17</v>
       </c>
       <c r="G21" s="101"/>
-      <c r="H21" s="75">
+      <c r="H21" s="76">
         <v>2.0</v>
       </c>
-      <c r="I21" s="75">
+      <c r="I21" s="76">
         <v>0.0</v>
       </c>
-      <c r="J21" s="75" t="s">
+      <c r="J21" s="76" t="s">
         <v>273</v>
       </c>
-      <c r="K21" s="74">
+      <c r="K21" s="75">
         <v>20.0</v>
       </c>
-      <c r="L21" s="75">
+      <c r="L21" s="76">
         <v>2.0</v>
       </c>
-      <c r="M21" s="75">
+      <c r="M21" s="76">
         <v>1.0</v>
       </c>
-      <c r="N21" s="75">
+      <c r="N21" s="76">
         <v>0.0</v>
       </c>
-      <c r="O21" s="75">
+      <c r="O21" s="76">
         <v>1.0</v>
       </c>
       <c r="P21" s="100">
         <v>4.0</v>
       </c>
-      <c r="Q21" s="2"/>
+      <c r="Q21" s="76"/>
     </row>
     <row r="22">
-      <c r="A22" s="71">
+      <c r="A22" s="72">
         <v>242.0</v>
       </c>
-      <c r="B22" s="75" t="s">
-        <v>539</v>
-      </c>
-      <c r="C22" s="75" t="s">
-        <v>540</v>
-      </c>
-      <c r="D22" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="75" t="s">
+      <c r="B22" s="76" t="s">
+        <v>559</v>
+      </c>
+      <c r="C22" s="76" t="s">
+        <v>560</v>
+      </c>
+      <c r="D22" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="76" t="s">
         <v>17</v>
       </c>
       <c r="G22" s="101"/>
-      <c r="H22" s="75">
+      <c r="H22" s="76">
         <v>2.0</v>
       </c>
-      <c r="I22" s="75">
+      <c r="I22" s="76">
         <v>0.0</v>
       </c>
-      <c r="J22" s="75" t="s">
+      <c r="J22" s="76" t="s">
         <v>286</v>
       </c>
-      <c r="K22" s="74">
+      <c r="K22" s="75">
         <v>21.0</v>
       </c>
-      <c r="L22" s="75">
+      <c r="L22" s="76">
         <v>2.0</v>
       </c>
-      <c r="M22" s="75">
+      <c r="M22" s="76">
         <v>3.0</v>
       </c>
-      <c r="N22" s="75">
+      <c r="N22" s="76">
         <v>3.0</v>
       </c>
-      <c r="O22" s="75">
+      <c r="O22" s="76">
         <v>1.0</v>
       </c>
       <c r="P22" s="100">
         <v>4.0</v>
       </c>
-      <c r="Q22" s="2"/>
+      <c r="Q22" s="76" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="71">
+      <c r="A23" s="72">
         <v>243.0</v>
       </c>
-      <c r="B23" s="75" t="s">
-        <v>541</v>
-      </c>
-      <c r="C23" s="75" t="s">
-        <v>542</v>
-      </c>
-      <c r="D23" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="75"/>
+      <c r="B23" s="76" t="s">
+        <v>561</v>
+      </c>
+      <c r="C23" s="76" t="s">
+        <v>562</v>
+      </c>
+      <c r="D23" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="76"/>
       <c r="G23" s="101"/>
-      <c r="H23" s="75">
+      <c r="H23" s="76">
         <v>2.0</v>
       </c>
-      <c r="I23" s="75">
+      <c r="I23" s="76">
         <v>0.0</v>
       </c>
-      <c r="J23" s="75" t="s">
+      <c r="J23" s="76" t="s">
         <v>299</v>
       </c>
-      <c r="K23" s="74">
+      <c r="K23" s="75">
         <v>22.0</v>
       </c>
-      <c r="L23" s="75">
+      <c r="L23" s="76">
         <v>2.0</v>
       </c>
-      <c r="M23" s="75">
+      <c r="M23" s="76">
         <v>3.0</v>
       </c>
-      <c r="N23" s="75">
+      <c r="N23" s="76">
         <v>2.0</v>
       </c>
-      <c r="O23" s="75">
+      <c r="O23" s="76">
         <v>2.0</v>
       </c>
       <c r="P23" s="100">
         <v>4.0</v>
       </c>
-      <c r="Q23" s="2"/>
+      <c r="Q23" s="76"/>
     </row>
     <row r="24">
-      <c r="A24" s="71">
+      <c r="A24" s="72">
         <v>244.0</v>
       </c>
-      <c r="B24" s="72" t="s">
-        <v>543</v>
-      </c>
-      <c r="C24" s="77" t="s">
-        <v>544</v>
-      </c>
-      <c r="D24" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="72" t="s">
+      <c r="B24" s="73" t="s">
+        <v>563</v>
+      </c>
+      <c r="C24" s="78" t="s">
+        <v>564</v>
+      </c>
+      <c r="D24" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="73" t="s">
         <v>17</v>
       </c>
       <c r="F24" s="97"/>
       <c r="G24" s="97"/>
-      <c r="H24" s="73">
+      <c r="H24" s="74">
         <v>2.0</v>
       </c>
       <c r="I24" s="98">
@@ -33819,35 +33945,37 @@
       <c r="J24" s="99" t="s">
         <v>312</v>
       </c>
-      <c r="K24" s="74">
+      <c r="K24" s="75">
         <v>23.0</v>
       </c>
-      <c r="L24" s="75">
+      <c r="L24" s="76">
         <v>2.0</v>
       </c>
-      <c r="M24" s="75">
+      <c r="M24" s="76">
         <v>1.0</v>
       </c>
-      <c r="N24" s="75">
+      <c r="N24" s="76">
         <v>0.0</v>
       </c>
-      <c r="O24" s="75">
+      <c r="O24" s="76">
         <v>1.0</v>
       </c>
       <c r="P24" s="100">
         <v>4.0</v>
       </c>
-      <c r="Q24" s="2"/>
+      <c r="Q24" s="76" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="78">
+      <c r="A25" s="79">
         <v>245.0</v>
       </c>
       <c r="B25" s="67" t="s">
-        <v>545</v>
-      </c>
-      <c r="C25" s="79" t="s">
-        <v>546</v>
+        <v>566</v>
+      </c>
+      <c r="C25" s="80" t="s">
+        <v>567</v>
       </c>
       <c r="D25" s="67" t="s">
         <v>17</v>
@@ -33857,7 +33985,7 @@
       <c r="G25" s="102" t="s">
         <v>110</v>
       </c>
-      <c r="H25" s="80">
+      <c r="H25" s="81">
         <v>2.0</v>
       </c>
       <c r="I25" s="94">
@@ -33866,143 +33994,149 @@
       <c r="J25" s="95" t="s">
         <v>325</v>
       </c>
-      <c r="K25" s="81">
+      <c r="K25" s="82">
         <v>24.0</v>
       </c>
-      <c r="L25" s="82">
+      <c r="L25" s="71">
         <v>3.0</v>
       </c>
-      <c r="M25" s="82">
+      <c r="M25" s="71">
         <v>1.0</v>
       </c>
-      <c r="N25" s="82">
+      <c r="N25" s="71">
         <v>0.0</v>
       </c>
-      <c r="O25" s="82">
+      <c r="O25" s="71">
         <v>1.0</v>
       </c>
       <c r="P25" s="103">
         <v>4.0</v>
       </c>
-      <c r="Q25" s="2"/>
+      <c r="Q25" s="71" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="71">
+      <c r="A26" s="72">
         <v>246.0</v>
       </c>
-      <c r="B26" s="75" t="s">
-        <v>547</v>
-      </c>
-      <c r="C26" s="75" t="s">
-        <v>548</v>
-      </c>
-      <c r="D26" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="75" t="s">
+      <c r="B26" s="76" t="s">
+        <v>569</v>
+      </c>
+      <c r="C26" s="76" t="s">
+        <v>570</v>
+      </c>
+      <c r="D26" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="76" t="s">
         <v>17</v>
       </c>
       <c r="G26" s="101"/>
-      <c r="H26" s="75">
+      <c r="H26" s="76">
         <v>2.0</v>
       </c>
-      <c r="I26" s="75">
+      <c r="I26" s="76">
         <v>0.0</v>
       </c>
-      <c r="J26" s="75" t="s">
+      <c r="J26" s="76" t="s">
         <v>338</v>
       </c>
-      <c r="K26" s="74">
+      <c r="K26" s="75">
         <v>25.0</v>
       </c>
-      <c r="L26" s="75">
+      <c r="L26" s="76">
         <v>2.0</v>
       </c>
-      <c r="M26" s="75">
+      <c r="M26" s="76">
         <v>1.0</v>
       </c>
-      <c r="N26" s="75">
+      <c r="N26" s="76">
         <v>0.0</v>
       </c>
-      <c r="O26" s="75">
+      <c r="O26" s="76">
         <v>1.0</v>
       </c>
       <c r="P26" s="104">
         <v>5.0</v>
       </c>
-      <c r="Q26" s="2"/>
+      <c r="Q26" s="76" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="71">
+      <c r="A27" s="72">
         <v>247.0</v>
       </c>
-      <c r="B27" s="72" t="s">
-        <v>549</v>
-      </c>
-      <c r="C27" s="77" t="s">
-        <v>550</v>
-      </c>
-      <c r="D27" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="77"/>
-      <c r="F27" s="72"/>
-      <c r="G27" s="72" t="s">
-        <v>551</v>
-      </c>
-      <c r="H27" s="73">
+      <c r="B27" s="73" t="s">
+        <v>571</v>
+      </c>
+      <c r="C27" s="78" t="s">
+        <v>572</v>
+      </c>
+      <c r="D27" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="78"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73" t="s">
+        <v>573</v>
+      </c>
+      <c r="H27" s="74">
         <v>2.0</v>
       </c>
-      <c r="I27" s="73">
+      <c r="I27" s="74">
         <v>0.0</v>
       </c>
       <c r="J27" s="87" t="s">
         <v>352</v>
       </c>
-      <c r="K27" s="74">
+      <c r="K27" s="75">
         <v>26.0</v>
       </c>
-      <c r="L27" s="75">
+      <c r="L27" s="76">
         <v>3.0</v>
       </c>
-      <c r="M27" s="75">
+      <c r="M27" s="76">
         <v>1.0</v>
       </c>
-      <c r="N27" s="75">
+      <c r="N27" s="76">
         <v>0.0</v>
       </c>
-      <c r="O27" s="75">
+      <c r="O27" s="76">
         <v>1.0</v>
       </c>
       <c r="P27" s="104">
         <v>5.0</v>
       </c>
-      <c r="Q27" s="2"/>
+      <c r="Q27" s="76" t="s">
+        <v>574</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="71">
+      <c r="A28" s="72">
         <v>248.0</v>
       </c>
-      <c r="B28" s="72" t="s">
-        <v>552</v>
-      </c>
-      <c r="C28" s="77" t="s">
-        <v>553</v>
-      </c>
-      <c r="D28" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="72" t="s">
+      <c r="B28" s="73" t="s">
+        <v>575</v>
+      </c>
+      <c r="C28" s="78" t="s">
+        <v>576</v>
+      </c>
+      <c r="D28" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="73" t="s">
         <v>17</v>
       </c>
       <c r="F28" s="105" t="s">
         <v>17</v>
       </c>
       <c r="G28" s="105"/>
-      <c r="H28" s="73">
+      <c r="H28" s="74">
         <v>2.0</v>
       </c>
       <c r="I28" s="106">
@@ -34011,47 +34145,47 @@
       <c r="J28" s="97" t="s">
         <v>366</v>
       </c>
-      <c r="K28" s="74">
+      <c r="K28" s="75">
         <v>27.0</v>
       </c>
-      <c r="L28" s="75">
+      <c r="L28" s="76">
         <v>2.0</v>
       </c>
-      <c r="M28" s="75">
+      <c r="M28" s="76">
         <v>1.0</v>
       </c>
-      <c r="N28" s="75">
+      <c r="N28" s="76">
         <v>0.0</v>
       </c>
-      <c r="O28" s="75">
+      <c r="O28" s="76">
         <v>2.0</v>
       </c>
       <c r="P28" s="104">
         <v>5.0</v>
       </c>
-      <c r="Q28" s="2"/>
+      <c r="Q28" s="76"/>
     </row>
     <row r="29">
-      <c r="A29" s="71">
+      <c r="A29" s="72">
         <v>249.0</v>
       </c>
       <c r="B29" s="105" t="s">
-        <v>554</v>
-      </c>
-      <c r="C29" s="77" t="s">
-        <v>555</v>
-      </c>
-      <c r="D29" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="72" t="s">
+        <v>577</v>
+      </c>
+      <c r="C29" s="78" t="s">
+        <v>578</v>
+      </c>
+      <c r="D29" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="73" t="s">
         <v>17</v>
       </c>
       <c r="F29" s="97" t="s">
         <v>17</v>
       </c>
       <c r="G29" s="97"/>
-      <c r="H29" s="73">
+      <c r="H29" s="74">
         <v>2.0</v>
       </c>
       <c r="I29" s="98">
@@ -34060,47 +34194,49 @@
       <c r="J29" s="99" t="s">
         <v>379</v>
       </c>
-      <c r="K29" s="74">
+      <c r="K29" s="75">
         <v>28.0</v>
       </c>
-      <c r="L29" s="75">
+      <c r="L29" s="76">
         <v>1.0</v>
       </c>
-      <c r="M29" s="75">
+      <c r="M29" s="76">
         <v>2.0</v>
       </c>
-      <c r="N29" s="75">
+      <c r="N29" s="76">
         <v>1.0</v>
       </c>
-      <c r="O29" s="75">
+      <c r="O29" s="76">
         <v>1.0</v>
       </c>
       <c r="P29" s="104">
         <v>5.0</v>
       </c>
-      <c r="Q29" s="2"/>
+      <c r="Q29" s="76" t="s">
+        <v>579</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="71">
+      <c r="A30" s="72">
         <v>250.0</v>
       </c>
-      <c r="B30" s="72" t="s">
-        <v>556</v>
-      </c>
-      <c r="C30" s="77" t="s">
-        <v>557</v>
-      </c>
-      <c r="D30" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="72" t="s">
+      <c r="B30" s="73" t="s">
+        <v>580</v>
+      </c>
+      <c r="C30" s="78" t="s">
+        <v>581</v>
+      </c>
+      <c r="D30" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="73" t="s">
         <v>17</v>
       </c>
       <c r="F30" s="97" t="s">
         <v>17</v>
       </c>
       <c r="G30" s="97"/>
-      <c r="H30" s="73">
+      <c r="H30" s="74">
         <v>2.0</v>
       </c>
       <c r="I30" s="98">
@@ -34109,192 +34245,194 @@
       <c r="J30" s="99" t="s">
         <v>392</v>
       </c>
-      <c r="K30" s="74">
+      <c r="K30" s="75">
         <v>29.0</v>
       </c>
-      <c r="L30" s="75">
+      <c r="L30" s="76">
         <v>3.0</v>
       </c>
-      <c r="M30" s="75">
+      <c r="M30" s="76">
         <v>3.0</v>
       </c>
-      <c r="N30" s="75">
+      <c r="N30" s="76">
         <v>3.0</v>
       </c>
-      <c r="O30" s="75">
+      <c r="O30" s="76">
         <v>3.0</v>
       </c>
       <c r="P30" s="104">
         <v>5.0</v>
       </c>
-      <c r="Q30" s="2"/>
+      <c r="Q30" s="76" t="s">
+        <v>582</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="78">
+      <c r="A31" s="79">
         <v>251.0</v>
       </c>
-      <c r="B31" s="82" t="s">
-        <v>558</v>
-      </c>
-      <c r="C31" s="82" t="s">
-        <v>559</v>
-      </c>
-      <c r="D31" s="82" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="82" t="s">
-        <v>17</v>
-      </c>
-      <c r="F31" s="82" t="s">
+      <c r="B31" s="71" t="s">
+        <v>583</v>
+      </c>
+      <c r="C31" s="71" t="s">
+        <v>584</v>
+      </c>
+      <c r="D31" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="71" t="s">
         <v>17</v>
       </c>
       <c r="G31" s="69"/>
-      <c r="H31" s="80">
+      <c r="H31" s="81">
         <v>2.0</v>
       </c>
       <c r="I31" s="107">
         <v>0.0</v>
       </c>
-      <c r="J31" s="82" t="s">
+      <c r="J31" s="71" t="s">
         <v>405</v>
       </c>
-      <c r="K31" s="81">
+      <c r="K31" s="82">
         <v>30.0</v>
       </c>
-      <c r="L31" s="82">
+      <c r="L31" s="71">
         <v>3.0</v>
       </c>
-      <c r="M31" s="82">
+      <c r="M31" s="71">
         <v>1.0</v>
       </c>
-      <c r="N31" s="82">
+      <c r="N31" s="71">
         <v>0.0</v>
       </c>
-      <c r="O31" s="82">
+      <c r="O31" s="71">
         <v>1.0</v>
       </c>
       <c r="P31" s="108">
         <v>5.0</v>
       </c>
-      <c r="Q31" s="2"/>
+      <c r="Q31" s="71"/>
     </row>
     <row r="32">
-      <c r="A32" s="71">
+      <c r="A32" s="72">
         <v>252.0</v>
       </c>
-      <c r="B32" s="75" t="s">
-        <v>560</v>
-      </c>
-      <c r="C32" s="75" t="s">
-        <v>561</v>
-      </c>
-      <c r="D32" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="F32" s="75" t="s">
+      <c r="B32" s="76" t="s">
+        <v>585</v>
+      </c>
+      <c r="C32" s="76" t="s">
+        <v>586</v>
+      </c>
+      <c r="D32" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="76" t="s">
         <v>17</v>
       </c>
       <c r="G32" s="2"/>
-      <c r="H32" s="73">
+      <c r="H32" s="74">
         <v>2.0</v>
       </c>
       <c r="I32" s="106">
         <v>0.0</v>
       </c>
-      <c r="J32" s="75" t="s">
+      <c r="J32" s="76" t="s">
         <v>418</v>
       </c>
-      <c r="K32" s="74">
+      <c r="K32" s="75">
         <v>31.0</v>
       </c>
-      <c r="L32" s="75">
+      <c r="L32" s="76">
         <v>1.0</v>
       </c>
-      <c r="M32" s="75">
+      <c r="M32" s="76">
         <v>1.0</v>
       </c>
-      <c r="N32" s="75">
+      <c r="N32" s="76">
         <v>0.0</v>
       </c>
-      <c r="O32" s="75">
+      <c r="O32" s="76">
         <v>1.0</v>
       </c>
       <c r="P32" s="109">
         <v>6.0</v>
       </c>
-      <c r="Q32" s="2"/>
+      <c r="Q32" s="76"/>
     </row>
     <row r="33">
-      <c r="A33" s="71">
+      <c r="A33" s="72">
         <v>253.0</v>
       </c>
-      <c r="B33" s="75" t="s">
-        <v>562</v>
-      </c>
-      <c r="C33" s="75" t="s">
-        <v>563</v>
-      </c>
-      <c r="D33" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="75" t="s">
+      <c r="B33" s="76" t="s">
+        <v>587</v>
+      </c>
+      <c r="C33" s="76" t="s">
+        <v>588</v>
+      </c>
+      <c r="D33" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="76" t="s">
         <v>17</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="73">
+      <c r="H33" s="74">
         <v>2.0</v>
       </c>
       <c r="I33" s="106">
         <v>0.0</v>
       </c>
-      <c r="J33" s="75" t="s">
+      <c r="J33" s="76" t="s">
         <v>431</v>
       </c>
-      <c r="K33" s="74">
+      <c r="K33" s="75">
         <v>32.0</v>
       </c>
-      <c r="L33" s="75">
+      <c r="L33" s="76">
         <v>1.0</v>
       </c>
-      <c r="M33" s="75">
+      <c r="M33" s="76">
         <v>2.0</v>
       </c>
-      <c r="N33" s="75">
+      <c r="N33" s="76">
         <v>0.0</v>
       </c>
-      <c r="O33" s="75">
+      <c r="O33" s="76">
         <v>1.0</v>
       </c>
       <c r="P33" s="109">
         <v>6.0</v>
       </c>
-      <c r="Q33" s="2"/>
+      <c r="Q33" s="76"/>
     </row>
     <row r="34">
-      <c r="A34" s="71">
+      <c r="A34" s="72">
         <v>254.0</v>
       </c>
-      <c r="B34" s="77" t="s">
-        <v>564</v>
-      </c>
-      <c r="C34" s="77" t="s">
-        <v>565</v>
-      </c>
-      <c r="D34" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" s="72" t="s">
+      <c r="B34" s="78" t="s">
+        <v>589</v>
+      </c>
+      <c r="C34" s="78" t="s">
+        <v>590</v>
+      </c>
+      <c r="D34" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="73" t="s">
         <v>17</v>
       </c>
       <c r="F34" s="110" t="s">
         <v>17</v>
       </c>
       <c r="G34" s="97"/>
-      <c r="H34" s="73">
+      <c r="H34" s="74">
         <v>2.0</v>
       </c>
       <c r="I34" s="98">
@@ -34303,96 +34441,100 @@
       <c r="J34" s="99" t="s">
         <v>444</v>
       </c>
-      <c r="K34" s="74">
+      <c r="K34" s="75">
         <v>33.0</v>
       </c>
-      <c r="L34" s="75">
+      <c r="L34" s="76">
         <v>2.0</v>
       </c>
-      <c r="M34" s="75">
+      <c r="M34" s="76">
         <v>3.0</v>
       </c>
-      <c r="N34" s="75">
+      <c r="N34" s="76">
         <v>1.0</v>
       </c>
-      <c r="O34" s="75">
+      <c r="O34" s="76">
         <v>2.0</v>
       </c>
       <c r="P34" s="109">
         <v>6.0</v>
       </c>
-      <c r="Q34" s="2"/>
+      <c r="Q34" s="76" t="s">
+        <v>591</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="71">
+      <c r="A35" s="72">
         <v>255.0</v>
       </c>
-      <c r="B35" s="75" t="s">
-        <v>566</v>
-      </c>
-      <c r="C35" s="75" t="s">
-        <v>567</v>
-      </c>
-      <c r="D35" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="F35" s="75" t="s">
+      <c r="B35" s="76" t="s">
+        <v>592</v>
+      </c>
+      <c r="C35" s="76" t="s">
+        <v>593</v>
+      </c>
+      <c r="D35" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="76" t="s">
         <v>17</v>
       </c>
       <c r="G35" s="2"/>
-      <c r="H35" s="73">
+      <c r="H35" s="74">
         <v>2.0</v>
       </c>
       <c r="I35" s="106">
         <v>0.0</v>
       </c>
-      <c r="J35" s="75" t="s">
+      <c r="J35" s="76" t="s">
         <v>457</v>
       </c>
-      <c r="K35" s="74">
+      <c r="K35" s="75">
         <v>34.0</v>
       </c>
-      <c r="L35" s="75">
+      <c r="L35" s="76">
         <v>2.0</v>
       </c>
-      <c r="M35" s="75">
+      <c r="M35" s="76">
         <v>1.0</v>
       </c>
-      <c r="N35" s="75">
+      <c r="N35" s="76">
         <v>0.0</v>
       </c>
-      <c r="O35" s="75">
+      <c r="O35" s="76">
         <v>1.0</v>
       </c>
       <c r="P35" s="109">
         <v>6.0</v>
       </c>
-      <c r="Q35" s="2"/>
+      <c r="Q35" s="76" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="71">
+      <c r="A36" s="72">
         <v>256.0</v>
       </c>
-      <c r="B36" s="72" t="s">
-        <v>568</v>
-      </c>
-      <c r="C36" s="77" t="s">
-        <v>569</v>
-      </c>
-      <c r="D36" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36" s="72" t="s">
+      <c r="B36" s="73" t="s">
+        <v>594</v>
+      </c>
+      <c r="C36" s="78" t="s">
+        <v>595</v>
+      </c>
+      <c r="D36" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="73" t="s">
         <v>17</v>
       </c>
       <c r="F36" s="110" t="s">
         <v>17</v>
       </c>
       <c r="G36" s="97"/>
-      <c r="H36" s="73">
+      <c r="H36" s="74">
         <v>2.0</v>
       </c>
       <c r="I36" s="98">
@@ -34401,35 +34543,37 @@
       <c r="J36" s="111" t="s">
         <v>470</v>
       </c>
-      <c r="K36" s="74">
+      <c r="K36" s="75">
         <v>35.0</v>
       </c>
-      <c r="L36" s="75">
+      <c r="L36" s="76">
         <v>3.0</v>
       </c>
-      <c r="M36" s="75">
+      <c r="M36" s="76">
         <v>1.0</v>
       </c>
-      <c r="N36" s="75">
+      <c r="N36" s="76">
         <v>0.0</v>
       </c>
-      <c r="O36" s="75">
+      <c r="O36" s="76">
         <v>1.0</v>
       </c>
       <c r="P36" s="109">
         <v>6.0</v>
       </c>
-      <c r="Q36" s="2"/>
+      <c r="Q36" s="76" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="78">
+      <c r="A37" s="79">
         <v>257.0</v>
       </c>
       <c r="B37" s="67" t="s">
-        <v>570</v>
-      </c>
-      <c r="C37" s="79" t="s">
-        <v>571</v>
+        <v>597</v>
+      </c>
+      <c r="C37" s="80" t="s">
+        <v>598</v>
       </c>
       <c r="D37" s="67" t="s">
         <v>17</v>
@@ -34441,7 +34585,7 @@
         <v>17</v>
       </c>
       <c r="G37" s="93"/>
-      <c r="H37" s="80">
+      <c r="H37" s="81">
         <v>2.0</v>
       </c>
       <c r="I37" s="94">
@@ -34450,41 +34594,43 @@
       <c r="J37" s="95" t="s">
         <v>483</v>
       </c>
-      <c r="K37" s="81">
+      <c r="K37" s="82">
         <v>36.0</v>
       </c>
-      <c r="L37" s="82">
+      <c r="L37" s="71">
         <v>3.0</v>
       </c>
-      <c r="M37" s="82">
+      <c r="M37" s="71">
         <v>3.0</v>
       </c>
-      <c r="N37" s="82">
+      <c r="N37" s="71">
         <v>3.0</v>
       </c>
-      <c r="O37" s="82">
+      <c r="O37" s="71">
         <v>2.0</v>
       </c>
       <c r="P37" s="112">
         <v>6.0</v>
       </c>
-      <c r="Q37" s="2"/>
+      <c r="Q37" s="71" t="s">
+        <v>599</v>
+      </c>
     </row>
     <row r="39">
       <c r="Q39" s="2"/>
     </row>
     <row r="40">
-      <c r="A40" s="73"/>
-      <c r="B40" s="75"/>
+      <c r="A40" s="74"/>
+      <c r="B40" s="76"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="73"/>
+      <c r="H40" s="74"/>
       <c r="I40" s="106"/>
       <c r="J40" s="2"/>
-      <c r="K40" s="73"/>
+      <c r="K40" s="74"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -34493,14 +34639,14 @@
       <c r="Q40" s="2"/>
     </row>
     <row r="41">
-      <c r="A41" s="73"/>
+      <c r="A41" s="74"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-      <c r="H41" s="73"/>
+      <c r="H41" s="74"/>
       <c r="I41" s="106"/>
       <c r="J41" s="2"/>
       <c r="K41" s="113"/>
@@ -34512,14 +34658,14 @@
       <c r="Q41" s="2"/>
     </row>
     <row r="42">
-      <c r="A42" s="73"/>
+      <c r="A42" s="74"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
-      <c r="H42" s="73"/>
+      <c r="H42" s="74"/>
       <c r="I42" s="106"/>
       <c r="J42" s="2"/>
       <c r="K42" s="113"/>
@@ -34531,17 +34677,17 @@
       <c r="Q42" s="2"/>
     </row>
     <row r="43">
-      <c r="A43" s="73"/>
+      <c r="A43" s="74"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
-      <c r="H43" s="73"/>
+      <c r="H43" s="74"/>
       <c r="I43" s="106"/>
       <c r="J43" s="2"/>
-      <c r="K43" s="73"/>
+      <c r="K43" s="74"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>

</xml_diff>